<commit_message>
Tested various responses to portfolio construction prompts
</commit_message>
<xml_diff>
--- a/data/Portfolio_construction_prompts.xlsx
+++ b/data/Portfolio_construction_prompts.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Personal documents\Github\FolioLLM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44ABEC4C-B9FE-4FAA-8A23-1A3F6DE42ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAE578D-73E6-4136-9D35-43C8566FE003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Prompt_test_results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="168">
   <si>
     <t>#</t>
   </si>
@@ -307,19 +308,703 @@
   </si>
   <si>
     <t>Invest in {number} ETFs which are targeting {"asset_class_focus"}?</t>
+  </si>
+  <si>
+    <t>Select {number} of ETFs for portfolio investing only in {"asset_class_focus"}?</t>
+  </si>
+  <si>
+    <t>Invest in {number_1} {strategy_1} ETFs, {number_2} {strategy_2} ETFs and {number_3} {strategy_3} ETFs equally?</t>
+  </si>
+  <si>
+    <t>Create a portfolio of {number} Funds with lowest Expense ratio?</t>
+  </si>
+  <si>
+    <t>Create a portfolio of {number} ETFs each with return between {ytd_return_1} and {ytd_return_2}?</t>
+  </si>
+  <si>
+    <t>Create a portfolio of {number} equal-weighted ETF investing in {geographical_composition}?</t>
+  </si>
+  <si>
+    <t>Create a portfolio of {number} equal-weighted ETF investing in {industry_sector}?</t>
+  </si>
+  <si>
+    <t>Construct a portfolio with investing {percent_1}% in {ticker_1}, {percent_2} in {ticker_2}, {percent_3} in {ticker_3} and {percent_4} in {ticker_4}?</t>
+  </si>
+  <si>
+    <t>Fingui2</t>
+  </si>
+  <si>
+    <t>ETFs</t>
+  </si>
+  <si>
+    <t>Sharpe</t>
+  </si>
+  <si>
+    <t>Sortino</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>ChatGPT4o</t>
+  </si>
+  <si>
+    <t>FolioLLM</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>To create a portfolio of three ETFs that invest in the United States, we can use an index fund or a combination of both. Here's an example of how you could construct a portfolio of three ETFs that invest in the technology sector, including stocks, bonds, and real estate investments. The choice between index funds and individual holdings depends on your risk tolerance, investment goals, and time horizon. For this example, we'll use a single index fund (ETF) to diversify across three sectors: technology, consumer discretionary, and energy. Each sector will have its own index composed of large-cap technology companies, mid-cap consumer discretionary companies, and small-cap energy companies. In addition to the index fund, we'll also include a mix of individual stocks from each sector to ensure some exposure to these specific industries. This portfolio provides a comprehensive view of the technology sector, which includes stocks, bonds, and real estate investments. By incorporating a mix of both index funds and individual holdings, investors can achieve a balance between cost, efficiency, and diversification, potentially leading to better long-term performance. It's important to note that individual stock selection should be based on thorough research, analysis, and valuation. A good starting point would be to evaluate the characteristics and growth potential of each sector, as well as its relative performance to the overall market. As with any investment strategy, it's crucial to regularly review and rebalance the portfolio to maintain desired asset allocation and mitigate risks.</t>
+  </si>
+  <si>
+    <t>As an AI language model, I cannot create a portfolio with specific investments that may not align with individual investors' preferences or risk tolerance. However, I can provide some general guidelines for constructing a diversified portfolio with ETFs in different countries. When constructing a portfolio with ETFs in South Korea and Japan, it's important to consider the potential for interest income, tax efficiency, and geopolitical stability. A portfolio that includes both emerging markets and developed markets would provide exposure to both growth opportunities and risk management strategies. Additionally, diversifying across geographic regions can help spread risk and minimize volatility over time. It's also crucial to understand the fees associated with each ETF, as they can impact returns and expense ratios. Ultimately, the decision of which countries to invest in is a complex one and requires careful consideration of individual circumstances. It's recommended to consult with a financial advisor or use online tools to create a customized investment plan tailored to your needs.</t>
+  </si>
+  <si>
+    <t>When investing in an ETF portfolio with three growth stocks and two value stocks and one blend ETF, it's important to consider the diversification of the investments and the potential impact on overall returns. In this case, you can achieve a balanced portfolio by allocating the majority to growth stocks (ETFs) and value stocks (ETFs), with a small portion allocated to a blend ETF that combines both growth and value themes. This approach allows for a more stable return profile while maintaining exposure to different asset classes based on risk tolerance and investment goals. It's important to note that the performance of these portfolios may vary over time, as the market experiences changes and opportunities arise. Regularly reviewing and rebalancing your portfolio is crucial to ensure alignment with your objectives and risk tolerance.</t>
+  </si>
+  <si>
+    <t>To create a portfolio of 5 ETFs each with a return between 10% and 20%, we can use the following formula: Return = (Number of EFPs * Expected Return) + (Number of S&amp;P 500 ETFs * S&amp;P 500 Return). Plugging in these values, our portfolio would be: 5 * (10% / 100) + 5 * (20% / 100) = 6.75 + 3.5 = 10.25%. This portfolio would provide a balanced return over time while considering market risk and other factors. As an AI language model, my goal is to provide objective, personalized advice that aligns with an individual's objectives and risk tolerance. However, it's important to note that the actual returns may vary based on various factors such as market conditions, tax implications, and geopolitical events. It's always recommended to conduct thorough research, compare prices, and consult with a financial advisor before making any investment decisions.</t>
+  </si>
+  <si>
+    <t>To create a portfolio of 5 equal-weighted ETFs investing in China, we can use the ETF symbol for the index, such as "CINQ." The following example creates a portfolio with 5 equities: 1 ETF (S&amp;P CINQ 500), 2 ETFs (Tibetan指数 ETFs), 3 ETFs (Shanghai Composite ETFs), and 4 ETFs (Chinese Unemployment Rate ETFs). Each ETF has an average expense ratio of around 1% per month, making it a cost-effective option for investors seeking to achieve a balanced portfolio. The portfolio is diversified across different sectors and asset classes to spread risks. As an investor, you can adjust the mix of investments based on your investment objectives, risk tolerance, and market conditions. Additionally, this portfolio provides exposure to the Shining Star Index, which is a well-diversified benchmark index that represents the performance of China's stock market over time.</t>
+  </si>
+  <si>
+    <t>S&amp;P CINQ 500 Equity, S&amp;P CINQ 500)</t>
+  </si>
+  <si>
+    <t>As an AI language model, I cannot provide investment advice or offer specific market indices. However, based on the choice of value-oriented funds in the industrial sector, some potential options include Vanguard Total Market Return ETF (TMQ) and Fidelity Industrial Stocks ETF (FIS). These funds aim to match the average returns of a broad market index with individual stocks held within each sector. Each fund offers exposure to different sectors and industries to cater to the varying risk-return profiles of individual investors.</t>
+  </si>
+  <si>
+    <t>To create an equal-weighted portfolio of ETFs with a minimum yield of 5%, we can use the following formula: Portfolio = 0.8 * EMA(ETF1) + 0.2 * EMA(ETF2) + ... + 0.3 * EMA(ETFn), where n is the number of ETFs in the portfolio. Plugging in the values, the portfolio would be: Portfolio = 0.8 * (12/100) + 0.2 * (12/100) + ... + 0.3 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100) + 0.2 * (12/100). Plugging in the values, the portfolio would be: Portfolio = 0.8 * (12 / 100) + 0.2 * (12 / 100) + ... + 0.3 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 / 100) + 0.2 * (12 /</t>
+  </si>
+  <si>
+    <t>As an AI language model, I cannot provide specific ETF holdings for individual investors or offer any trading strategies. However, I can provide general guidelines on what each ETF might include based on popular choices. Each ETF may also have unique characteristics or features that make it suitable for specific markets or sectors. As with any investment decision, it's important to evaluate the fund's performance, fees, and other relevant factors before making an investment decision. It's also advisable to consider your own risk tolerance and investment goals when selecting ETFs.</t>
+  </si>
+  <si>
+    <t>An optimal portfolio that maximizes Sharpe Ratio should consist of 70% of assets invested in the United States and 30% in non-U.S. markets, such as Europe or Japan. This strategy ensures that the portfolio's risk is aligned with its potential returns while minimizing volatility. Additionally, diversification through asset allocation can reduce overall portfolio risk. It's important to note that the Sharpe Ratio is just one measure of portfolio performance, and it may not accurately reflect the portfolio's long-term sustainability. Investors should use other factors to assess the performance of their portfolios, such as turnover rates and fees.</t>
+  </si>
+  <si>
+    <t>TMQ, FIS</t>
+  </si>
+  <si>
+    <t>As an AI language model, I do not have access to the individual fund portfolios recommended by the user, but I can provide some general guidelines for mean variance optimization for such portfolios based on historical data and analysis techniques used in portfolio optimization.
+Mean Variance (MVA) optimization involves identifying systematic risks and systematically removing them from the portfolio to improve risk-adjusted returns over time. In the context of market index funds or ETFs, this may involve subtracting the market index from the fund's target asset allocation to reduce volatility. By optimizing mean variance through MVA, investors can enhance their portfolio resilience against adverse market movements and achieve more consistent long-term returns. It's important to note that mean variance optimization alone does not guarantee superior performance, as other factors such as the underlying assets and the investor's investment strategy also play a significant role in determining portfolio success.</t>
+  </si>
+  <si>
+    <t>As an AI language model, I cannot provide specific investment advice, but I can offer some general guidelines for constructing a portfolio of 5 ETFs with equal weightings based on your individual risk tolerance, investment goals, and market conditions. It's important to note that the weighting of your ETFs may vary based on factors like market capitalization, dividend yields, and inflation trends. A more balanced approach would involve diversifying across different asset classes with a mix of equities, fixed-income securities, and alternative investments. You should also consider factors such as time horizons, liquidity needs, and tax implications when determining the appropriate level of exposure. Consulting with a financial advisor or using a chart-based tool like Morningstar can help you create a comprehensive investment strategy tailored to your individual circumstances.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Creating a balanced and diversified portfolio of exchange-traded funds (ETFs) involves selecting ETFs that cover different asset classes, regions, and sectors. Here is a portfolio of 5 ETFs with equal weights, each covering different aspects of the market:
+Vanguard Total Stock Market ETF (VTI)
+Asset Class: U.S. Total Market
+Description: Provides exposure to the entire U.S. equity market, including small-, mid-, and large-cap growth and value stocks.
+iShares MSCI Emerging Markets ETF (EEM)
+Asset Class: Emerging Markets Equity
+Description: Offers exposure to stocks from emerging market economies, providing growth potential and diversification.
+iShares Core U.S. Aggregate Bond ETF (AGG)
+Asset Class: U.S. Bonds
+Description: Tracks an index of U.S. investment-grade bonds, providing a stable income stream and reducing portfolio volatility.
+Vanguard FTSE Developed Markets ETF (VEA)
+Asset Class: International Developed Markets Equity
+Description: Provides exposure to a broad range of companies in developed markets outside of the U.S.
+SPDR Gold Shares (GLD)
+Asset Class: Commodities (Gold)
+Description: Tracks the price of gold, offering a hedge against inflation and market volatility.
+Portfolio Construction
+Each ETF will have an equal weight of 20% in the portfolio.
+VTI: 20%
+EEM: 20%
+AGG: 20%
+VEA: 20%
+GLD: 20%
+Rationale
+Diversification: The portfolio covers a range of asset classes (equities, bonds, commodities) and regions (U.S., international developed markets, emerging markets).
+Risk Management: The inclusion of bonds and gold helps to mitigate risk and provide stability.
+Growth Potential: Exposure to emerging markets and developed international markets alongside the U.S. market offers growth opportunities.
+This portfolio is designed to provide a balanced approach, capturing the benefits of diversification while managing risk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating a portfolio of 3 ETFs that invest solely in the United States requires careful selection to ensure diversification across different sectors and market caps. Here is a recommended portfolio with equal weights:
+Vanguard Total Stock Market ETF (VTI)
+Asset Class: U.S. Total Market
+Description: Provides exposure to the entire U.S. equity market, including small-, mid-, and large-cap growth and value stocks.
+SPDR S&amp;P 500 ETF Trust (SPY)
+Asset Class: U.S. Large-Cap Stocks
+Description: Tracks the performance of the S&amp;P 500 Index, representing 500 of the largest companies in the U.S. economy.
+iShares Russell 2000 ETF (IWM)
+Asset Class: U.S. Small-Cap Stocks
+Description: Provides exposure to small-cap stocks, offering potential for higher growth compared to large-cap stocks.
+Portfolio Construction
+Each ETF will have an equal weight of 33.33% in the portfolio.
+VTI: 33.33%
+SPY: 33.33%
+IWM: 33.33%
+Rationale
+Diversification: The portfolio covers different segments of the U.S. stock market (total market, large-cap, and small-cap).
+Growth Potential: By including both large-cap (SPY) and small-cap (IWM) ETFs, the portfolio balances stability with growth opportunities.
+Market Coverage: VTI ensures comprehensive exposure across all market caps and sectors, while SPY and IWM provide focused investments in large and small companies, respectively.
+This portfolio aims to capture the broad performance of the U.S. market while taking advantage of the growth potential of smaller companies and the stability of larger companies.
+</t>
+  </si>
+  <si>
+    <t>Portfolio with 5 ETFs Investing in South Korea
+iShares MSCI South Korea ETF (EWY)
+Asset Class: South Korean Equities
+Description: Provides exposure to large and mid-sized companies in South Korea.
+Franklin FTSE South Korea ETF (FLKR)
+Asset Class: South Korean Equities
+Description: Tracks the FTSE South Korea RIC Capped Index, covering large and mid-cap South Korean stocks.
+Global X MSCI Korea ETF (KORU)
+Asset Class: South Korean Equities
+Description: Seeks to provide investment results that correspond generally to the price and yield performance of the MSCI Korea 25/50 Index.
+First Trust Korea AlphaDEX Fund (FKO)
+Asset Class: South Korean Equities
+Description: Tracks the NASDAQ AlphaDEX South Korea Index, which selects stocks from the South Korean market based on growth factors.
+Xtrackers MSCI South Korea Hedged Equity ETF (DBKO)
+Asset Class: South Korean Equities (Currency Hedged)
+Description: Offers exposure to the South Korean equity market while hedging against currency fluctuations between the USD and KRW.
+Portfolio with 3 ETFs Investing in Japan
+iShares MSCI Japan ETF (EWJ)
+Asset Class: Japanese Equities
+Description: Provides exposure to large and mid-sized companies in Japan.
+Franklin FTSE Japan ETF (FLJP)
+Asset Class: Japanese Equities
+Description: Tracks the FTSE Japan RIC Capped Index, covering large and mid-cap Japanese stocks.
+WisdomTree Japan Hedged Equity Fund (DXJ)
+Asset Class: Japanese Equities (Currency Hedged)
+Description: Offers exposure to Japanese equities while hedging against fluctuations in the yen.
+Portfolio Construction
+To ensure equal weighting within each regional portfolio, the construction will be as follows:
+South Korea Portfolio:
+EWY: 20%
+FLKR: 20%
+KORU: 20%
+FKO: 20%
+DBKO: 20%
+Japan Portfolio:
+EWJ: 33.33%
+FLJP: 33.33%
+DXJ: 33.33%
+Rationale
+South Korea Portfolio:
+Diversification: The selection includes broad market exposure, growth-focused, and currency-hedged options.
+Market Coverage: The ETFs provide comprehensive exposure to South Korean equities, covering large and mid-cap stocks.
+Japan Portfolio:
+Diversification: Combines broad market exposure with a currency-hedged option to mitigate yen fluctuations.
+Market Coverage: Ensures broad exposure to Japanese equities, focusing on large and mid-cap stocks.
+By diversifying within each country's market and including currency-hedged options, this portfolio aims to capture growth opportunities while managing risk related to currency fluctuations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portfolio Construction with Growth, Value, and Blend ETFs
+3 Growth ETFs
+Vanguard Growth ETF (VUG)
+Asset Class: U.S. Growth Equities
+Description: Focuses on U.S. large-cap growth stocks, providing exposure to companies with high growth potential.
+iShares Russell 1000 Growth ETF (IWF)
+Asset Class: U.S. Growth Equities
+Description: Tracks the Russell 1000 Growth Index, covering large and mid-cap U.S. growth stocks.
+ARK Innovation ETF (ARKK)
+Asset Class: U.S. Growth Equities
+Description: Invests in companies focused on disruptive innovation, offering high growth potential in various sectors such as technology, genomics, and fintech.
+2 Value ETFs
+Vanguard Value ETF (VTV)
+Asset Class: U.S. Value Equities
+Description: Provides exposure to U.S. large-cap value stocks, focusing on companies that are undervalued compared to their fundamentals.
+iShares Russell 1000 Value ETF (IWD)
+Asset Class: U.S. Value Equities
+Description: Tracks the Russell 1000 Value Index, covering large and mid-cap U.S. value stocks.
+1 Blend ETF
+iShares Core S&amp;P Total U.S. Stock Market ETF (ITOT)
+Asset Class: U.S. Blend Equities
+Description: Provides exposure to the entire U.S. stock market, including large, mid, and small-cap stocks, balancing growth and value investments.
+Portfolio Allocation
+Each ETF will be equally weighted in the portfolio.
+Growth ETFs:
+VUG: 16.67%
+IWF: 16.67%
+ARKK: 16.67%
+Value ETFs:
+VTV: 16.67%
+IWD: 16.67%
+Blend ETF:
+ITOT: 16.67%
+Rationale
+Growth ETFs: Selected to provide exposure to high-growth potential stocks, targeting sectors and companies with strong growth trajectories.
+Value ETFs: Focus on undervalued companies with strong fundamentals, offering stability and potential for capital appreciation.
+Blend ETF: Offers comprehensive market exposure, balancing both growth and value stocks to provide a diversified foundation for the portfolio.
+This portfolio aims to capture the benefits of both growth and value investing while maintaining a balanced exposure to the broader market.
+</t>
+  </si>
+  <si>
+    <t>Creating a portfolio of ETFs with historical returns between 10% and 20% can be challenging, as past performance is not always indicative of future results. However, I can suggest a diversified mix of ETFs that have demonstrated strong historical performance within that range. Please note that returns can vary over different time periods and market conditions.
+Portfolio of 5 ETFs with Historical Returns Between 10% and 20%
+Invesco QQQ Trust (QQQ)
+Asset Class: U.S. Large-Cap Growth
+Description: Tracks the Nasdaq-100 Index, which includes 100 of the largest non-financial companies listed on the Nasdaq Stock Market.
+Historical Return: ~15-20% (over the past decade)
+Vanguard Information Technology ETF (VGT)
+Asset Class: U.S. Sector - Technology
+Description: Provides exposure to information technology stocks, a sector known for high growth potential.
+Historical Return: ~15-20% (over the past decade)
+iShares MSCI USA Momentum Factor ETF (MTUM)
+Asset Class: U.S. Momentum Stocks
+Description: Tracks the performance of large and mid-cap U.S. stocks exhibiting relatively higher price momentum.
+Historical Return: ~12-18% (over the past decade)
+SPDR S&amp;P 500 Growth ETF (SPYG)
+Asset Class: U.S. Large-Cap Growth
+Description: Tracks the S&amp;P 500 Growth Index, which includes stocks with growth characteristics within the S&amp;P 500.
+Historical Return: ~12-16% (over the past decade)
+iShares MSCI Emerging Markets ETF (EEM)
+Asset Class: Emerging Markets Equity
+Description: Provides exposure to large and mid-sized companies in emerging market countries.
+Historical Return: ~10-15% (over the past decade)
+Portfolio Allocation
+Each ETF will be equally weighted in the portfolio.
+QQQ: 20%
+VGT: 20%
+MTUM: 20%
+SPYG: 20%
+EEM: 20%
+Rationale
+Diversification: The portfolio covers different sectors (technology, growth, momentum) and regions (U.S. and emerging markets).
+Growth Potential: The selected ETFs have historically strong returns, driven by high-growth sectors and market segments.
+Risk Management: While the focus is on growth, the inclusion of a broad emerging markets ETF adds geographical diversification, which can help mitigate risk.
+This portfolio aims to achieve balanced growth by investing in ETFs with a track record of strong returns, while ensuring diversification across different sectors and regions.</t>
+  </si>
+  <si>
+    <t>Creating a portfolio of value ETFs that focus specifically on the industrial sector can provide exposure to companies that are considered undervalued relative to their fundamentals within this sector. Here are five such ETFs, each focusing on industrials and generally following a value investment strategy:
+Portfolio of 5 Value ETFs Focusing on the Industrial Sector
+Industrial Select Sector SPDR Fund (XLI)
+Asset Class: U.S. Industrial Sector
+Description: Tracks the performance of the industrial sector of the S&amp;P 500 Index, covering a range of industries including aerospace, defense, machinery, and transportation.
+iShares U.S. Industrials ETF (IYJ)
+Asset Class: U.S. Industrial Sector
+Description: Provides exposure to U.S. companies in the industrial sector, including manufacturers and distributors of capital goods, providers of commercial services, and transportation services.
+Vanguard Industrials ETF (VIS)
+Asset Class: U.S. Industrial Sector
+Description: Tracks the performance of the MSCI US Investable Market Industrials 25/50 Index, which includes stocks of U.S. companies within the industrial sector.
+Fidelity MSCI Industrials Index ETF (FIDU)
+Asset Class: U.S. Industrial Sector
+Description: Seeks to provide investment returns that correspond to the performance of the MSCI USA IMI Industrials Index.
+First Trust Industrials/Producer Durables AlphaDEX Fund (FXR)
+Asset Class: U.S. Industrial Sector
+Description: Follows the StrataQuant Industrials Index, which employs a quant-based methodology to select industrials stocks with strong value characteristics.
+Portfolio Allocation
+Each ETF will be equally weighted at 20%.
+XLI: 20%
+IYJ: 20%
+VIS: 20%
+FIDU: 20%
+FXR: 20%
+Rationale
+Sector Focus: All selected ETFs concentrate on the industrial sector, ensuring targeted exposure.
+Value Orientation: The chosen ETFs are designed to include companies that are undervalued based on fundamental metrics, aligning with a value investment strategy.
+Diversification within Sector: While all ETFs focus on the industrial sector, they track different indices and may have slightly different methodologies, offering some diversification within the sector.
+This portfolio aims to capitalize on the potential for value appreciation within the industrial sector by investing equally in ETFs that target undervalued companies across various industries within the sector.</t>
+  </si>
+  <si>
+    <t>Portfolio of 5 Equal-Weighted ETFs Investing in China
+iShares MSCI China ETF (MCHI)
+Asset Class: Chinese Equities
+Description: Provides exposure to large and mid-sized companies in China, covering a broad spectrum of sectors.
+KraneShares CSI China Internet ETF (KWEB)
+Asset Class: Chinese Technology and Internet
+Description: Focuses on Chinese companies operating in the internet and technology sectors, offering exposure to high-growth industries.
+SPDR S&amp;P China ETF (GXC)
+Asset Class: Chinese Equities
+Description: Tracks the S&amp;P China BMI Index, covering a wide range of Chinese companies across various sectors and market capitalizations.
+Xtrackers Harvest CSI 300 China A-Shares ETF (ASHR)
+Asset Class: Chinese A-Shares
+Description: Invests in A-shares, which are shares of mainland China-based companies that trade on the Shanghai and Shenzhen stock exchanges.
+Invesco China Technology ETF (CQQQ)
+Asset Class: Chinese Technology
+Description: Provides exposure to Chinese technology companies, including those in the technology hardware, software, and services sectors.
+Portfolio Allocation
+Each ETF will be equally weighted at 20%.
+MCHI: 20%
+KWEB: 20%
+GXC: 20%
+ASHR: 20%
+CQQQ: 20%
+Rationale
+Diversification: The portfolio includes a mix of broad market ETFs (MCHI, GXC) and sector-specific ETFs (KWEB, CQQQ), as well as different share classes (ASHR for A-shares).
+Growth Potential: Focuses on high-growth sectors such as technology and internet, which are significant drivers of China's economic expansion.
+Market Coverage: Provides comprehensive exposure to various segments of the Chinese market, from large-cap to A-shares and technology sectors.
+This portfolio aims to capture the broad potential of China's economy by diversifying across different sectors and market capitalizations, while maintaining a focus on high-growth industries.</t>
+  </si>
+  <si>
+    <t>Portfolio of High-Yield ETFs
+iShares U.S. Preferred Stock ETF (PFF)
+Asset Class: Preferred Stocks
+12-Month Yield: ~6.0%
+Description: Invests in U.S. preferred stocks, offering higher yields compared to common equities.
+SPDR Bloomberg Barclays High Yield Bond ETF (JNK)
+Asset Class: High-Yield Bonds
+12-Month Yield: ~5.5%
+Description: Tracks an index of high-yield corporate bonds, providing substantial income.
+iShares J.P. Morgan USD Emerging Markets Bond ETF (EMB)
+Asset Class: Emerging Markets Bonds
+12-Month Yield: ~5.3%
+Description: Focuses on U.S. dollar-denominated bonds issued by emerging market governments and corporations.
+Global X SuperDividend ETF (SDIV)
+Asset Class: Global Dividend Stocks
+12-Month Yield: ~7.0%
+Description: Invests in 100 of the highest dividend-yielding equity securities in the world.
+Vanguard Real Estate ETF (VNQ)
+Asset Class: Real Estate Investment Trusts (REITs)
+12-Month Yield: ~5.2%
+Description: Provides exposure to U.S. REITs, which typically offer higher yields.
+Portfolio Allocation
+Each ETF will be equally weighted at 20%.
+PFF: 20%
+JNK: 20%
+EMB: 20%
+SDIV: 20%
+VNQ: 20%
+Rationale
+Income Generation: All selected ETFs offer a 12-month yield of at least 5%, ensuring the portfolio meets the high-income criterion.
+Diversification: The portfolio includes a mix of preferred stocks, high-yield bonds, emerging markets bonds, global dividend stocks, and REITs, reducing sector-specific risks.
+Yield Stability: These ETFs are known for their focus on income generation, providing relatively stable yields compared to more volatile growth-focused investments.
+This portfolio aims to provide a steady income stream while maintaining diversification across different asset classes and regions.</t>
+  </si>
+  <si>
+    <t>Creating a diversified portfolio with ETFs focusing on different asset groups can help balance risk and return. Here are five ETFs, each representing a different asset group:
+Portfolio of 5 ETFs Focusing on Different Asset Groups
+Vanguard Total Stock Market ETF (VTI)
+Asset Class: U.S. Equities
+Description: Provides exposure to the entire U.S. stock market, including small-, mid-, and large-cap growth and value stocks.
+iShares MSCI ACWI ex U.S. ETF (ACWX)
+Asset Class: International Equities
+Description: Offers exposure to large and mid-cap companies across developed and emerging markets outside of the U.S.
+Vanguard Total Bond Market ETF (BND)
+Asset Class: U.S. Bonds
+Description: Tracks the performance of the Bloomberg Barclays U.S. Aggregate Float Adjusted Index, covering investment-grade bonds.
+iShares TIPS Bond ETF (TIP)
+Asset Class: Inflation-Protected Bonds
+Description: Provides exposure to U.S. Treasury Inflation-Protected Securities (TIPS), which help protect against inflation.
+SPDR Gold Shares (GLD)
+Asset Class: Commodities (Gold)
+Description: Tracks the price of gold, offering a hedge against inflation and market volatility.
+Portfolio Allocation
+Each ETF will be equally weighted at 20%.
+VTI: 20%
+ACWX: 20%
+BND: 20%
+TIP: 20%
+GLD: 20%
+Rationale
+Diversification: The portfolio includes a mix of U.S. and international equities, U.S. bonds, inflation-protected securities, and commodities.
+Risk Management: Combining different asset classes helps manage risk by reducing the impact of any single asset class underperforming.
+Inflation Protection: The inclusion of TIPS and gold provides protection against inflation, enhancing the portfolio's stability.
+This portfolio aims to provide broad diversification across different asset groups, balancing potential growth with risk management.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating an optimal portfolio with the highest Sharpe ratio involves selecting a mix of ETFs that provide the best risk-adjusted returns. The Sharpe ratio measures the excess return per unit of risk. Here is a suggested portfolio focused on U.S. assets, aiming to maximize the Sharpe ratio based on historical data:
+Optimal Portfolio with High Sharpe Ratio
+Vanguard Total Stock Market ETF (VTI)
+Asset Class: U.S. Equities
+Description: Provides exposure to the entire U.S. stock market, including small-, mid-, and large-cap growth and value stocks.
+Vanguard Dividend Appreciation ETF (VIG)
+Asset Class: U.S. Dividend Growth Stocks
+Description: Focuses on companies with a strong track record of increasing dividends, which tend to be more stable and less volatile.
+iShares MSCI USA Quality Factor ETF (QUAL)
+Asset Class: U.S. Quality Stocks
+Description: Invests in large- and mid-cap U.S. stocks with strong fundamentals, such as high return on equity, stable earnings growth, and low financial leverage.
+iShares 7-10 Year Treasury Bond ETF (IEF)
+Asset Class: U.S. Treasury Bonds
+Description: Provides exposure to U.S. Treasury bonds with maturities between 7 and 10 years, offering stability and low correlation to equities.
+iShares U.S. Real Estate ETF (IYR)
+Asset Class: U.S. Real Estate
+Description: Tracks an index of U.S. real estate investment trusts (REITs) and other real estate-related stocks, providing diversification and income.
+Portfolio Allocation
+To achieve an optimal balance, the portfolio can be weighted as follows, based on historical data and risk-adjusted return analysis:
+VTI: 30%
+VIG: 25%
+QUAL: 20%
+IEF: 15%
+IYR: 10%
+Rationale
+Diversification: This portfolio includes a mix of equities (total market, dividend growth, and quality stocks), bonds, and real estate, providing broad market exposure and diversification.
+Risk Management: The inclusion of U.S. Treasury bonds helps reduce overall portfolio volatility, while dividend growth and quality stocks tend to be less volatile and provide stable returns.
+High Sharpe Ratio: By combining assets with high expected returns and low correlations, this portfolio aims to achieve a high Sharpe ratio, maximizing risk-adjusted returns.
+Steps to Construct and Monitor the Portfolio
+Historical Data Analysis: Use historical return, risk, and correlation data to estimate the expected return and volatility for each ETF.
+Optimization Model: Implement a mean-variance optimization model to determine the asset weights that maximize the Sharpe ratio.
+Periodic Rebalancing: Regularly rebalance the portfolio (e.g., quarterly or annually) to maintain the target asset allocation and adapt to changing market conditions.
+This approach aims to provide a well-balanced, high-performing portfolio tailored to the U.S. market, focusing on maximizing risk-adjusted returns.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimal Portfolio Weights
+Optimal Portfolio Weights and Performance
+Based on the mean-variance optimization performed, here are the optimal weights for the ETFs and the portfolio's performance metrics:
+Optimal Portfolio Weights
+ETF	Weight
+VTI	0.00%
+VIG	0.00%
+QUAL	0.00%
+IEF	0.00%
+IYR	100.00%
+Portfolio Performance
+Annualized Return: 8.49%
+Annualized Volatility: 15.62%
+Sharpe Ratio: 0.42
+Interpretation
+Concentration in IYR: The optimization suggests investing fully in the iShares U.S. Real Estate ETF (IYR), indicating that this ETF provided the highest risk-adjusted return among the selected options based on the sample data.
+Sharpe Ratio: The Sharpe ratio of 0.42 indicates a moderate risk-adjusted return. While the return is attractive, the portfolio is highly concentrated in one asset, which might not align with typical diversification principles.
+To ensure a more diversified approach while maintaining a high Sharpe ratio, consider re-evaluating the ETF selection or adjusting the constraints and objectives of the optimization model. ​​
+The optimization was performed using a sample dataset of 5 years of daily returns. Here is a summary of the time period and data used:
+Time Period: 5 years
+Frequency: Daily returns
+ETFs: VTI, VIG, QUAL, IEF, IYR
+Since we used simulated data due to the limitations of this environment, the exact dates are illustrative. In a real-world scenario, the specific start and end dates would be from January 1, 2018, to January 1, 2023.
+For more accurate and relevant optimization, it's recommended to use real historical price data for the mentioned ETFs over the desired time period.
+</t>
+  </si>
+  <si>
+    <t>Here's a suggested portfolio with 3 ETFs investing in the United States? They are well-diversified and can potentially provide some income and capital appreciation over time. Please note that this is just one possible portfolio and may not include all suitable ETFs and their weightings based on your individual needs and risk tolerance. It's recommended to thoroughly research and consider your investment goals, time horizon, and risk tolerance when constructing your ETFs and portfolio. You can use the following ETFs and their weights in the portfolio: iShares S&amp;P 50001000 DB Real Estate UCITS ETF: 33.33%, Purpose Global Bond Fund: 33.33%, BlackRock TESLA Digital TPS 50 ETF: 33.33%. It's also important to keep in mind that investing always carries some level of risk, and it's crucial to thoroughly understand the fund's strategies, fees, and composition before adding them to your portfolio. This ETFs and others like it do not participate in your portfolio and will not be reflected. I suggest reviewing the list of ETFs and their weights in the portfolio further to ensure that they align with your investment objectives and risk tolerance levels. Additionally, you might want to consider adding some more low-cost index funds or ETFs to manage any portfolio concentration issues.</t>
+  </si>
+  <si>
+    <t>Here is a suggested portfolio with 5 ETFs investing in South Korea and 3 ETFs investing in Japan? You can see the following ETFs and their weights in the portfolio: 469160 KIMAX株学・テクノロジー・モバイル株式価格基金: 25.00%, KIMAX株学・モバイル事業積極見通基金: 25.00%, KIMAX株学・テクノロジー事業積極見通基金: 25.00%, KIMAX株学セグメント動向担当社KIMACE 日本メイコルデューデリジェンステクノロジーやモバイル ETF: 25.00%, KIMACESpoke 日本銭政務部門テクノロジーや金融サービス分野の指数を活用して構成する証券ETF: 25.00%更大
+Please note that this is just one possible ETF list and there may be other suitable ETFs and strategies for your portfolio. It is recommended to review the ETFs and their weights carefully and consider your investment goals, time horizon, and risk tolerance before adding any additional ETFs or strategies to the portfolio. It also makes sense to consider consulting with a financial advisor if you have specific investment objectives or risk tolerance needs.</t>
+  </si>
+  <si>
+    <t>Here is a list of suitable ETFs and their weightings:
+FGO MSCI Emerging Markets Free Press Index 40 Exchange Traded Fund
+FGO Global Mainframe Technology 40 Exchange Traded Fund
+FGO Global New貌 40 Exchange Traded Fund
+FGO S&amp;P/AMR Warren 50 ETF
+Fondo de Inverso GIP A STree ETP: High Dividend
+iShares World Equity High Income UCITS ETF
+NextGen Post-Brexit 40 Exchange Traded Fund
+Practional allocations to Global Equity Strategies
+First Trust Bloomberg Lightweight Investment Grade ETF
+Xtrackers MSCI Class I Daily exchange-traded fund
+Xtrackers US Equity High Dividend ETF
+YLETF 4D S&amp;P 500: 4x Short
+YLETF 4A S&amp;P 500 Currency Hedged: 4x Short
+Please note that this is not an exhaustive list and some of the above-mentioned ETFs may have negative weightings or may be excluded from the list due to their weightage in the S&amp;P 500 or other relevant indices. It's also important to consider your individual investment objectives, time horizon, and risk tolerance when selecting an ETFs.</t>
+  </si>
+  <si>
+    <t>To create a portfolio with 5 ETFs that meet your criteria, we can use the following ETFs and their weights as follows: CCB Global ETN: 10.00%, Leverage Shares -3x Short UBS ETP Securities: 10.00%, CCB Global ETN: 10.00%, MTEK ETF Leaders Tech: 10.00%, CCB Global ETN: 10.00%, Hwabao WP CSI 500 Leaders ETF: 10.00% (10.00% is 10% not just 10% added, you need to see the ETF and see if it's truly 10% or more) - I am including this ETF because it has higher weightings to technology than most other stocks. In terms of asset allocation, we have a portfolio with 94.67% longs and 1.33% shortens to maintain our desired balance of long and short positions. Let me know if you require any further assistance.</t>
+  </si>
+  <si>
+    <t>Here is an ETF portfolio with 5 ETFs investing in China? The following ETFs can be added to the portfolio: 512310 DIYib Crude Oil Bollinger Benches 2x Inverse: 512310 DIYib Crude Oil Bollinger Benches 2x Inverse is an ETF managed by Global X Asia Pacific. 512310 DIYib CSI 500 in Energy: 512310 DIYibCSI BABA Business Division is an ETF managed by Global X Asia Global. 512310 DIYib CSI 500 in Consumer Discretionary: 512310 DIYib CSI 500 in Healthcare is an ETF managed by Global X Asia Europe. 512310 DIYib CSI 500 in Technology: 512310 DIYib CSI 500 in New Materials is an ETF managed by Global X Asia China. 512310 DIYib CSI 500 in Internet and Online: 512310 DIYib CSI 500 in Financials is an ETF managed by Global X Asia China. This ETF portfolio includes 5 ETFs investing in China. It is made up of 5 ETFs that pay a consistent tracking fee: 512310 DIYib Crude Oil Bollinger Benches 2x Inverse: 512310 DIYib CSI 500 in Energy: 512310 DIYib CSI 500 in Healthcare: 512310 DIYib CSI 500 in Consumer Discretionary: 512310 DIYib CSI 500 in New Materials: 512310 DIYib CSI 500 in Internet and Online: 512310 DIYib CSI 500 in Financials: holding 51.23% of the portfolio. The weightings for each ETF are as follows: 512310 DIYib Crude Oil Bollinger Benches 2x Inverse: 100.00%, 512310 DIYib CSI 500 in Energy: 100.00%, 512310 DIYib CSI 500 in Healthcare: 100.00%, 512310 DIYib CSI 500 in Consumer Discretionary: 100.00%, 512310 DIYib CSI 500 in New Materials: 100.00%, 512310 DIYib CSI 500 in Internet and Online: 100.00%. The next ETF in the portfolio is 512310 DIYib CSI 500 in Energy. Here is the updated ETF portfolio: 512310 DIYib Crude Oil Bollinger Benches 2x Inverse: 512310 DIYib CSI 500 in Energy 1h4w Inverse: 512310 DIYib CSI 500 in Energy 1X Daily 2x Inverse: 512310 DIYib CSI 500 in Energy 1d/2d 2x Inversed: 512310 DIYib CSI 500 in Energy 1xDaily 3x Inverse: 512310 DIYib CSI 500 in Energy 1X Daily 3a: 512310 DIYib CSI 500 in Energy 1T/TC 2x Inverse: 512310 DIYib CSI 500 in Energy 1xT 2X Inverse: 512310 DIYib CSI 500 in Energy 1h4w T 50: 512310 DIYib CSI 500 in Energy 1T/TC 2x Inverse: 512310 DIYib CSI 500 in Energy 1T 3x Inverse: 512310 DIYib CSI 500 in Energy 1xDaily 3a: 512310 DIYib CSI 500 in Energy 1T/TC 2x Inverse: 512310 DIYib CSI 500 in Energy 1T 3x Inverse: 512310 DIYib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To create an investment strategy with the desired mix of Value ETFs, we can follow these steps: 1. Add 5 ETFs investing in Industrial? Answer: 5.0
+2. only buy shares of these ETFs, not other categories: IEDGI - International电讯设备制造商指数 ETF
+3. Careful selection of the right sectors and indexes: IVEC - Intellectual Property Value Index ETF
+4. Diversify across more than 5 ETFs: IVEC - Intellectual Property Value Index ETF - weightings for other technology themes: -1x, -1x, 1x, 10x, 20x
+Please see the following table to confirm the allocation and weightings:
+ETF	Weightings
+IEDGI - International电讯设备制造商指数 ETF	5.00%
+IVEC - Intellectual Property Value Index ETF	5.00%
+IVEC - Intellectual Property Value Index ETF + Large Cap Technology MSCI ESG Leaders ETF H: 5.00%	5.00%
+IVEC - Intellectual Property Value Index ETF + Large Cap IT: 5.00%	5.00%
+Please note that	</t>
+  </si>
+  <si>
+    <t>To create an equal-weighted portfolio with 12 million shares holding 12-month simple interest payments, we can use the following ETFs and their weightings:
+EQAL - Invesco Russell 1000 Equal Weight ETF: 12,000,000 shares, 9.87%, 5.67%
+WNXT40 - 10X Wealth Next40 Equal Weighted ETF: 12,000,000 shares, 9.87%, 5.67%
+RSP - Invesco S&amp;P 500 Equal-Weight ETF: 12,000,000 shares, 9.87%, 5.67% (for the S&amp;P 500 Index) or 3,625,000 shares, 5.67% (for the US Treasury 10+ Index), 5.67% (for the S&amp;P 500 10 plus Index), 5.67% (for the US Treasury 20+ Index), 5.67% (for the Dow Jones Industrial 20 plus Index), 5.67% (for the U.S. Treasury 10 plus 20 plus Index), 5.67% (for the U.S. Treasury 20 plus 20 plus Index), 5.67% (for the U.S. Treasury 10 plus 30 plus Index), 5.67% (for the U.S. Treasury 30 plus Index), 5.67% (for the U.S. Treasury 100 plus Index), 5.67% (for the U.S. Treasury 30 plus Index), 5.67% (for the U.S. Treasury 100 plus 30 plus Index), 5.67% (for the U.S. Treasury 20 plus Index), 5.67% (for the U.S. Treasury 20 plus 30 plus Index), 5.67% (for the U.S. Treasury 30 plus Index), 5.67% (for the U.S. Treasury 100 plus Index), 5.67% (for the U.S. Treasury 30 plus Index), 5.67% (for the U.S. Treasury 100 plus 20 plus Index), 5.67% (for the U.S. Treasury 20 plus 20 plus Index), 5.67% (for the U.S. Treasury 100 plus Index), 5.67% (for the U.S. Treasury 30 plus Index), 5.67% (for the U.S. Treasury 100 plus 30 plus Index). This portfolio has an average daily return of 5.67% and an average weekly return of 5.67%. As it does not include any high-dividend-yield stocks, we have selected these ETFs as potential high-yield options. However, please note that this is just one possible weighting and that other factors such as sector diversification, management experience, and market position may influence the portfolio's weightings. As an AI language model, I cannot provide specific buy or sell orders without more information about your investment objectives, risk tolerance, and trading style. It's also important to consider consulting with a financial advisor before making investment decisions.</t>
+  </si>
+  <si>
+    <t>Here is a list of 5 ETFs with unique investment themes and expense ratios that can be combined to form a multi-ETF? Please see the following ETFs and their weightings:
+KB KBSTAR Active Korea Total Bond Market AA- ETF: 20.00%, 25.00%,
+iShares World Equity High Income UCITS ETF: 20.00%, 25.00%,
+TF通风 Power Index - Short, Tachlit Composite Power Index - Long, Global UBS ETC: 20.00%, 25.00%,
+YLETF 4A S&amp;P 500 Currency Hedged: 20.00%, 25.00%,
+YLETF 4D S&amp;P 500, United States: 20.00%, 25.00%,
+Please note that this is not an exhaustive list, and there may be other ETFs or strategies that could be added to meet the needs of your investment objectives and risk tolerance. It's also important to consider the specific ETFs and their weights within your portfolio before investing.</t>
+  </si>
+  <si>
+    <t>To create an optimal portfolio with the highest Sharpe ratio, we can consider adding the following ETFs and their weights:
+iShares US 10+ Year Treasury Bond 98% TA-98: 12.50%, 47.33% in portfolio
+YLETF 4D S&amp;P 500: 12.50%, 47.33% in portfolio
+YLETF 4A S&amp;P 500 Currency Hedged: 12.50%, 47.33% in portfolio
+YLETF 4D Nasdaq 100: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 Currency Hedged: 12.50%, 47.33% in portfolio
+YLETF 4Dallerian MSCI ESG: 12.50%, 47.33% in portfolio
+YLETF 4Aallerian MSCI ESG Daily 2X Leveraged: 12.50%, 47.33% in portfolio
+YLETF 4D Nasdaq 100 Currency Hedged: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 Currency Hedged: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 + 3x Long Hwamans Securities: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 + 3X Short Huabansas Securities: 12.50%, 47.33% in portfolio
+YLETF 4A NASDAQ 100 1-13ta-ESPA: 12.50%, 47.33% in portfolio
+YLETF 4D Nasdaq 100 1-13ta: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 13fa ta FIBO: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 13fa -100a: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 13a -100c: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 13b -13btf: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 13bb -13ba: 12.50%, 47.33% in portfolio
+YLETF 4A NASDAQ 100 13b -100a: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 13a: 12.50%, 47.33% in portfolio
+YLETF 4A NASDAQ 100 13b: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 13a: 12.50%, 47.33% in portfolio
+YLETF 4D Nasdaq 100 13a: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 13da: 12.50%, 47.33% in portfolio
+YLETF 4D Nasdaq 100 13de: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 13dea: 12.50%, 47.33% in portfolio
+YLETF 4A Nasdaq 100 13db: 12.50%, 47.3</t>
+  </si>
+  <si>
+    <t>As per your request, I have performed mean/variance optimization (MVO) on the list of funds and generated an optimized portfolio with low correlation and high volatility. The following is the optimized portfolio with minimal correlation and 98.3% level of volatility:
+INQQ - INQQ India Internet &amp; Ecommerce ESG-S UCITS ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+CSYU - CSIF IE MSCI USA Tech 125 ESG Universal Blue UCITS ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+SPMV Invesco S&amp;P 500 Minimum Variance ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+Invesco S&amp;P 500 - 2x Daily High Dividend Yield UCITS ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+Invesco S&amp;P 500 2X Daily Low Volatility UCITS ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+iShares Global Equity 1.35X Daily Inverse UCITS ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+Invesco US 500 Daily Inverse UCITS ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM指数 - 1D IT/IT服务业 ESG ETC UCITS ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Asia IT/IT服务业 ESG ETC UCITS ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Europe IT/IT服务业 ESG ETC UCITS ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+CMC Global Technology 125 ESG Universal Active 125 UCits ETF: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Global Technology 125 ESG Universal 2x Daily 2x Live: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Global Technology 125 ESG 125 Daily 2X Inverse: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Global ESG 125 125 Daily 2X Inverse: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Global ESG 125 2X Inverse 2X 125 Daily: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Global ESG 125 2X Inverse 2X 125: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Global ESG 125 2X Inverse 2X 125 Daily 2X Inverse: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Global ESG 125 2X Inverse 2X 125 Daily 2X Daily: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Global ESG 125 2X Inverse 2X 125 Daily 2X High: 70.00%, 11.14% annual return, 6.56% spot volatility
+CCM Global ESG 125 2X Inverse 2X 125 Daily 2X High Dividend: 70.00%, 11.14% annual return,</t>
+  </si>
+  <si>
+    <t>Sure, here's an ETF portfolio with 5 ETFs investing in South Korea, consisting of:
+Samsung KODEX Active Korea Total Bond Market AA- ETF
+Samsung KODEX ItNext时金通指数期货期权 ETF
+Samsung KODEX itNext时金通指数期货期权 ETF - High Income
+Samsung KODEXITN时引式指数期货商品ETF
+*三星堆EXOP不起眼指数-先知ETF
+Samsung KODEX ITN韩国领先指数期货商品ETF</t>
+  </si>
+  <si>
+    <t>The Invesco FTSE RAFI US 1000 UCITS ETF focuses on theUSA, uses None, and has fund assets totaling 463.27. It trades under the ticker R1RUZ, has an average bid-ask spread of 0.49%, and follows a Dynamic Allocation strategy. It trades under the ticker R1RUZ, has a year-to-date return of +11.27%. A portfolio of 5 ETFs with a 0%, focusing on United States, and having a 0%. It trades under the ticker R1RUZ, has an average bid-ask spread of 0.49%, and follows a Dynamic Allocation strategy. The Invesco FTSE RAFI US 1000 UCITS ETF has fund assets totaling 463.27, uses None, and has a NAV tracking error of 0.0286%. It trades under the ticker R1RUZ, has a NAV tracking error of 0.0286%, and follows a Dynamic Allocation strategy. The Invesco FTSE RAFI US 1000 UCITS ETF has fund assets totaling 463.27, uses None, and has a NAV tracking error of 0.0286%. It focuses on theUSA region, follows a Dynamic Allocation strategy, and has a fund type of ETF. It can be found on the Invesco FTSE RAFI US 1000 UCITS ETF portfolio. It has a NAV tracking error of 0.0286%, a 10-year volume of 266122, and a return month-to-date of +11.27%. A portfolio of 5 ETFs with a total fund assets of 463.27, a fund type of ETF, and an expense ratio of 0.20%. It can be found on the Invesco FTSE RAFI US 1000 UCITS ETF portfolio. It has a NAV tracking error of 0.0286%, a 10-year volume of 266122, and a return month-to-date of +11.27%. A fund with a similar trade target date of 07/13/17, class assets totaling 463.27, and a return month-to-date of +11.27%. The Invesco FTSE RAFI US 1000 UCITS ETF has fund assets totaling 463.27, uses None, and has a NAV tracking error of 0.0286%. It focuses on theUSA region, follows a Dynamic Allocation strategy, and has a fund type of ETF. It can be found on the Invesco FTSE RAFI US 1000 UCITS ETF portfolio. It has a NAV tracking error of 0.0286%, a 10-year volume of 266122, and a return month-to-date of +11.27%. The Invesco FTSE RAFI US 1000 UCITS ETF has fund assets totaling 463.27, a fund type of ETF, and an expense ratio of 0.20%. It can be found on the Invesco FTSE RAFI US 1000 UCITS ETF portfolio. It has a NAV tracking error of 0.0286%, a 10-year volume of 266122, and a return month-to-date of +11.27%. The Invesco FTSE RAFI US 1000 UCITS ETF has fund assets totaling 463.27, uses None, and has a NAV tracking error of 0.0286%. It focuses on theUSA region, follows a Dynamic Allocation strategy, and has a fund type of ETF. It can be found on the Invesco FTSE RAFI US 1000 UCITS ETF portfolio. It has a NAV tracking error of 0.0286%, a 10-year volume of 266122, and a return month-to-date of +11.27%. The Invesco FTSE RAFI US 1000 UCITS ETF has fund assets totaling 463.27, a fund type of ETF, and an expense ratio of 0.20%. It can be found on the Invesco FTSE RAFI US 1000 UCITS ETF portfolio. It has a NAV tracking error of 0.0286%, a 10-year volume of 266122, and a</t>
+  </si>
+  <si>
+    <t>The V FMK-US Equity Factor Rotation ETF focuses on the United States region, specifically targeting the Blend strategy, and has fund assets totaling 196.07. It has a NAV tracking error of 5.2481%, a 30-day volume of 10823, and a return month-to-date of +3.22%. The FNB MidCap ETF is a regular trade move back to this resource. It has a NAV tracking error of 5.2481%, a 30-day volume of 10823, and a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to optimize the FNB MidCap ETF's 0.51%, target fund assets of 196.07, and a return month-to-date of +3.22%. It trades under the ticker VNMSF. It has a combination type of Multi-Strategy, an average bid-ask spread of 0.60%, and a year-to-date return of +11.16%. The V FMK-US Equity Factor Rotation ETF focuses on the United States region, primarily targeting the Blend strategy, and has fund assets totaling 196.07. It has a NAV tracking error of 5.2481%, a 30-day volume of 10823, and a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to optimize the FNB MidCap ETF's 0.51%, focuses on the United States region, specifically targeting the Blend strategy, and has a NAV tracking error of 5.2481%. It has a mix taker type, a 30-day volume of 10823, and a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to improve the FNB MidCap ETF's 0.51%, focuses on the United States region, follows a Blend strategy, and has a return month-to-date of +3.22%. It trades under the ticker VNMSF. It has a combination type of Multi-Strategy, has a NAV tracking error of 5.2481%, and has a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF focuses on the United States region, primarily targeting the Blend strategy, and has fund assets totaling 196.07. It has a combination type of Multi-Strategy, has a NAV tracking error of 5.2481%, and has a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to optimize the FNB MidCap ETF's 0.51%, focuses on the United States region, specifically targeting the Blend strategy, and has a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to improve the FNB MidCap ETF's 0.51%, focuses on the United States region, follows a Blend strategy, and has a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to enhance the FNB MidCap ETF's 0.51%, focuses on the United States region, follows a Blend strategy, and has a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to maximize the FNB MidCap ETF's 0.51%, focuses on the United States region, and follows a Blend strategy. It has a combination type of Multi-Strategy, has a NAV tracking error of 5.2481%, and has a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to optimize the FNB MidCap ETF's 0.51%, focuses on the United States region, specifically targeting the Blend strategy, and has a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to improve the FNB MidCap ETF's 0.51%, focuses on the United States region, follows a Blend strategy, and has a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to enhance the FNB MidCap ETF's 0.51%, focuses on the United States region, follows a Blend strategy, and has a return month-to-date of +3.22%. The V FMK-US Equity Factor Rotation ETF aims to maximize the FNB MidCap ETF's 0.51%, focuses on the United States region, and follows a Blend strategy. It has a combination type of Multi-Strategy, has</t>
+  </si>
+  <si>
+    <t>The Korea Investment KINDEX Japan Semiconductor ETF has 56.7, is managed by Korea Investment Holdings Co L, and focuses on the Japan region. It has a fund type of ETF. The portfolio includes 469160, has an average bid-ask spread of 0.23%, and follows a Blend strategy. The 168580 focuses on the Japan region, uses derivatives (N), and has a NAV tracking error of None. The Korea Investment KINDEX Japan Semiconductor ETF has fund assets totaling 469160, a 30-day volume of 172746, and a return month-to-date of +1.88%. It has a 1y return month-to-date of +2.15%, and a 30-day return month-to-date of +3.26%. The KIM Ace Japan Semiconductor ETF is associated with the Japan Region, follows a Blend strategy, and has a NAV tracking error of None. It trades under the ticker 284400. The Korea Investment KINDEX Japan Semiconductor ETF has fund assets totaling 469160, a 30-day volume of 172746, and a return month-to-date of +3.26%. In contrast, the Korea Investment KINDEX Japan Semiconductor ETF focuses on the Japan region, uses derivatives (N), and has a NAV tracking error of None. It trades under the ticker 284400. As a result, the Korea Investment KINDEX Japan Semiconductor ETF has fund assets totaling 469160, a 30-day volume of 172746, and a return month-to-date of +3.26%. It follows a Blend strategy, has a fund type of ETF, and has a NAV tracking error of None. On a whole, the Korea Investment KINDEX Japan Semiconductor ETF holds a combination type of Derivative, has an average bid-ask spread of 0.23%, and follows a Blend strategy. It trades under the ticker 284400. However, the Korea Investment KINDEX Japan Semiconductor ETF has fund assets totaling 469160, a 30-day volume of 172746, and a return month-to-date of +3.26%. It follows a Blend strategy, uses derivatives (N), and has a NAV tracking error of None. Despite its N.A., the Korea Investment KINDEX Japan Semiconductor ETF has fund assets totaling 469160, a 30-day volume of 172746, and a return month-to-date of +3.26%. It maintains a combination type of Derivative, has an average bid-ask spread of 0.23%, and follows a Blend strategy. On a whole, the Korea Investment KINDEX Japan Semiconductor ETF holds a combination type of Derivative, has a average bid-ask spread of 0.23%, and follows a Blend strategy. It trades under the ticker 284400. While it has fund assets totaling 469160, it has a 30-day volume of 172746, and a return month-to-date of +3.26%. It follows a Blend strategy, has a fund type of ETF, and has a NAV tracking error of None. Despite its N.A., the Korea Investment KINDEX Japan Semiconductor ETF holds fund assets totaling 469160, a 30-day volume of 172746, and a return month-to-date of +3.26%. It maintains a combination type of Derivative, has an average bid-ask spread of 0.23%, and follows a Blend strategy. It trades under the ticker 284400. In contrast, the Korea Investment KINDEX Japan Semiconductor ETF focuses on the Japan Region, uses derivatives (N), and has a NAV tracking error of None. It trades under the ticker 284400. Despite its N.A., the Korea Investment KINDEX Japan Semiconductor ETF holds fund assets totaling 469160, a 30-day volume of 172746, and a return month-to-date of +3.26%. It follows a Blend strategy, has a fund type of Derivative, has an average bid-ask spread of 0.23%, and follows a Blend strategy. It trades under the ticker 284400. Despite its N.A., the Korea Investment KINDEX Japan Semiconductor ETF holds fund assets totaling 469160, a 30-day volume of 172746, and a return month-to-date of +3.</t>
+  </si>
+  <si>
+    <t>To find an ETF with a +0.67%, focuses on N.A., and focuses on Broad Market, we need to know what these ETFs have a 0.11%, target date of 09/09/15, and how it has a None. We can use the Fidelity International Low Volatility Factor ETF. It has a NAV tracking error of None, a 30-day volume of 464364, and a return month-to-date of +2.79%. We're looking for a fund that has a 11.18%, focuses on N.A., and is managed by Grace Partners of DuPage LP. To find an ETF with a 0.16%, focuses on N.A., and follows a Blend strategy? The Fidelity International Low Volatility Factor ETF would be a good choice, using a fund type of ETF, an average bid-ask spread of 0.32%, and a year-to-date return of +11.13%. It has a NAV tracking error of None, a 30-day volume of 464364, and a return month-to-date of +2.79%. As for the Fidelity International Low Volatility Factor ETF, it has a NAV tracking error of 0.16%, focuses on the N.A. region, and follows a Blend strategy. It can be having a one-day return of +11.18%. If you were interested in an ETF with a 0.16%, focuses on the N.A. region, and follows a Blend strategy, we might consider the Fidelity International Low Volatility Factor ETF. It has a NAV tracking error of None, uses a fund type of ETF, and has a return month-to-date of +2.79%. In terms of the 3 Growth ETFs, 2 Value ETFs, and 1 Blend ETF, it has a NAV tracking error of 0.16%, focuses on the N.A. region, and follows a Blend strategy. It can be achieved with a fund type of ETF, has a NAV tracking error of None, and follows a 1-day return of +11.18%. If you wanted to engage with this fund, you might consider the Fidelity International Low Volatility Factor ETF. It has a NAV tracking error of 0.16%, focuses on the N.A. region, and follows a Blend strategy. It can be used by FMR LLC, has a NAV tracking error of 0.16%, and follows a 1-day return of +11.18%. If you wanted to explore an ETF with a 0.16%, focuses on the N.A. region, and follows a Blend strategy, you might consider the Fidelity International Low Volatility Factor ETF. It has a NAV tracking error of None, focuses on the N.A. region, and follows a Blend strategy. It can be achieved with a fund type of ETF, has a NAV tracking error of 0.16%, and follows a 1-day return of +11.18%. If you did not find a match to the Fidelity International Low Volatility Factor ETF, you might consider the Fidelity International Low Volatility Factor ETF. It has a NAV tracking error of None, focuses on the N.A. region, and follows a Blend strategy. It can be used by FMR LLC, has a NAV tracking error of 0.16%, and follows a 1-day return of +11.18%. If you wanted to explore an ETF with a 0.16%, focuses on the N.A. region, and follows a Blend strategy, you might consider the Fidelity International Low Volatility Factor ETF. It has a NAV tracking error of None, focuses on the N.A. region, and follows a Blend strategy. It can be used by FMR LLC, has a NAV tracking error of 0.16%, and follows a 1-day return of +11.18%. If you wanted to learn about the Fidelity International Low Volatility Factor ETF, it would be a good fit, using a fund type of ETF, has a NAV tracking error of None, and follows a 1-day return of +11.18%. If you wanted to explore an ETF with a 0.16%, focuses on the N.A. region, and follows a Blend strategy, you might consider the Fidelity International Low Volatility Factor ETF. It has a NAV tracking error of None, focuses on the N.A. region, and follows a Blend strategy. It can be accessed by FMR LLC, has a NAV tracking error of 0.16%, and follows a 1-day return of +11.18%. If you wanted to explore an ETF</t>
+  </si>
+  <si>
+    <t>A balanced, N.A., and N.A. style ETF would be a good fit for this�uter. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It trades under the ticker JPTN, has an average bid-ask spread of 0.24%, and follows a Dynamic Allocation strategy. It has a 15/24/23. It has a 1.00%, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a Balanced strategy, focuses on the N.A. asset class, and has a NAV tracking error of None. It trades under the ticker JPTN, has an average bid-ask spread of 0.24%, and follows a Conservative Allocation strategy. It has a15/24/23 style ETF. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.21%. It follows a N.A. style. It has a NAV tracking error of None, a 30-day volume of 47690.25, and a return month-to-date of +2.2</t>
+  </si>
+  <si>
+    <t>he ChinaAMC CSI 100 ETF is a portfolio of 5 equal-weighted ETF investing in China. It has fund assets totaling 512380, an expense ratio of 0%, and trades under the ticker 560050. The ETF focuses on the China region, specifically targeting the N.A. industry, and follows a Blend strategy. It has fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. The ChinaAMC CSI 100 ETF has a NAV tracking error of None. It has a 3.17%, a 30-day volume of 40767, and a return month-to-date of +1.10%. It has a 30-day volume of 40767, a return month-to-date of +1.10%, and a NAV tracking error of None. The ChinaAMC CSI 100 ETF focuses on the China region, specifically targeting the N.A. industry, and follows a Blend strategy. It has fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a NAV tracking error of None, a 30-day volume of 40767, and a return month-to-date of +1.10%. It has a NAV tracking error of None, a 30-day volume of 40767, and a return month-to-date of +1.10%. The ChinaAMC CSI 100 ETF focuses on the China region, specifically targeting the N.A. industry, and follows a Blend strategy. It has fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a NAV tracking error of None, a 30-day volume of 40767, and a return month-to-date of +1.10%. It has a NAV tracking error of None, a 30-day volume of 40767, and a return month-to-date of +1.10%. The ChinaAMC CSI 100 ETF focuses on the China region, specifically targeting the N.A. industry, and follows a Blend strategy. It has fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a NAV tracking error of None, a 30-day volume of 40767, and a return month-to-date of +1.10%. The ChinaAMC CSI 100 ETF focuses on the China region, specifically targeting the N.A. industry, and follows a Blend strategy. It has fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and at least 80% of non-cash assets in constituent stocks. It has a fund assets totaling 90% of total assets and</t>
+  </si>
+  <si>
+    <t>he XLI - Industrial Select Sector SPDR Fund is a good choice, considering its Industrial Select Sector SPDR Fund. It trades under the ticker NXLU, has an average bid-ask spread of 0.23%, and follows a Value strategy. Therefore, it might be a good fit for investors looking for a particular asset class. The Fund focuses on the Industrial Select Sector index, uses a concentrated approach, and focuses on the Industrial Sector. To ensure a match, the XLI - Industrial Select Sector SPDR Fund would be a good choice, following a Value strategy. It has fund assets totaling 567.11, was incepted in 05/22/17, and follows a Value strategy. In terms of the XLI - Industrial Select Sector SPDR Fund, it has a number of peers, is managed by X-Square Capital LLC, and follows a Value strategy. If you have a similar fund with a None style, we can assume that it has a 0.29%. A more specific question about this fund is "Invest equally into 5 Value ETFs focusing on Industrial sector." It has a NAV tracking error of 0.2819%, a 30-day volume of 417342.09, and a return month-to-date of +3.54%. It has a NAV tracking error of 0.0416%, a 30-day volume of 417342.09, and a return month-to-date of +3.54%. To match this fund's Industrial Select Sector, investors can consider investing in the XLI - Industrial Select Sector SPDR Fund. It has a type of ETF, has aisinorized value strategy, and follows a Value strategy. It has a few competitors, is managed by X-Square Capital LLC, and follows a Value strategy. Since the XLI - Industrial Select Sector SPDR Fund has options. It has a NAV tracking error of 0.29%, a 30-day volume of 417342.09, and a return month-to-date of +3.54%. In terms of the XLI - Industrial Select Sector SPDR Fund, it has a similar fund with a type of ETF, is managed by X-Square Capital LLC, and follows a Value strategy. If you have a similar fund with a相同 format, it can be predicted that it has a NAV tracking error of 0.29%. A more specific question about this fund is "Invest equally into 5 Value ETFs focusing on Industrial sector." It has a type of ETF, has a IPAC configuration of 0.29%, a 30-day volume of 417342.09, and a return month-to-date of +3.54%. It has a NAV tracking error of 0.29%, a 30-day volume of 417342.09, and a return month-to-date of +3.54%. It has a similar fund with a type of ETF, is managed by X-Square Capital LLC, and follows a Value strategy. Since the XLI - Industrial Select Sector SPDR Fund has options. It has a IPAC configuration of 0.29%, a 30-day volume of 417342.09, and a return month-to-date of +3.54%. To match this fund's Industrial Select Sector, investors can consider investing in the XLI - Industrial Select Sector SPDR Fund. It has a type of ETF, has a IPAC configuration of 0.29%, a 30-day volume of 417342.09, and a return month-to-date of +3.54%. It has a similar fund with a format, is managed by X-Square Capital LLC, and follows a Value strategy. It has a 30-day volume of 417342.09. As a comparable fund, it focuses on the Industrial Select Sector, uses a IPAC configuration of 0.29%, focuses on the Industrial Select Sector, and is managed by X-Square Capital LLC. It has a NAV tracking error of 0.29%. A more specific question about this fund is "Invest equally into 5 Value ETFs focusing on Industrial sector". It has a type of ETF, has a IPAC configuration of 0.29%, a 30-day volume of 417342.09, and a return month-to-date of +3.54%. It has a similar fund with a format, is managed by X-Square Capital LLC, and follows a Value strategy. It has a 30-day volume of 4
+Textbox
+Type your message here...</t>
+  </si>
+  <si>
+    <t>The SPDR S&amp;P 500 Equal Weight ETF is a good choice, using the Invesco S&amp;P 1000 Equal Weight ETF. It has a fund type of ETF, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. A similar fund with a None style would be N.A., having a 10/10/08. It has a total fund assets of 79.92, an expense ratio of 0.20%, and trades under the ticker WNXT40. It has a 12M value accepted, a 30-day volume of 22744, and a return month-to-date of +1.93%. If you're looking for a fund with a None style, the SPDR S&amp;P 500 Equal Weight ETF might be what you're looking for. It has a NAV tracking error of 0.3504%, a 30-day volume of 22744, and a return month-to-date of +1.93%. If you have a specific question about this ETN, it's worth noting that it has a fund type of ETF, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. A similar fund with a None style would be N.A., having a NAV tracking error of 10/10/08. It has a total fund assets of 79.92, an expense ratio of 0.20%, and trades under the ticker WNXT40. It has a fund type of ETF, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. If you're interested in a fund with a None style, the SPDR S&amp;P 500 Equal Weight ETF would be a good fit, using the Invesco S&amp;P 1000 Equal Weight ETF. It has a fund type of ETF, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. If you have a specific question about this ETN, it's worth noting that it has a fund type of ETN, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. A similar fund with a None style would be N.A., having a NAV tracking error of 10/10/08. It has a total fund assets of 79.92, an expense ratio of 0.20%, and trades under the ticker WNXT40. If you have a specific question about this ETN, it's worth noting that it has a fund type of ETN, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. If you're looking for a fund with a None style, the SPDR S&amp;P 500 Equal Weight ETF would be a good fit, using the Invesco S&amp;P 1000 Equal Weight ETF. It has a fund type of ETF, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. A similar fund with a None style would be N.A., having a fund type of ETN, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. A similar fund with a None style would be N.A., focusing on the Invesco S&amp;P 1000 Equal Weight ETF. It has a fund type of ETN, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. If you have a specific question about this ETN, it's worth noting that it has a fund type of ETN, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. A similar fund with a None style would be N.A., focusing on the Invesco S&amp;P 1000 Equal Weight ETF. It has a fund type of ETN, an average bid-ask spread of 0.39%, and a year-to-date return of +10.62%. A similar fund with a None style would be N.A., targeting the Invesco S&amp;P 500 Equal Weight ETF. It has a fund type of ETN, an average bid-ask spread of 0.39%, and a year-to-date return of +1</t>
+  </si>
+  <si>
+    <t>The Capital Group US Multi-Sector Income ETF focuses on the United States region, specifically targeting the Investment Grade sector, and is associated with the Fixed Income it targets. It has fund assets totaling 106.32, an expense ratio of 0.47%, and trades under the ticker CGMS. As such, it follows a Corporate strategy and maintains a None style. It has相关的 ETFs including AVPS, ACI, and a related id. It has a NAV tracking error of 2.9817%, a 30-day volume of 11612, and a return month-to-date of +1.25%. To maintain a N.A., the Capital Group US Multi-Sector Income ETF has a 1.98%. On a若您 need, the Capital Group US Multi-Sector Income ETF focuses on the Investment Grade region, follows a Corporate strategy, and has a NAV tracking error of 2.9817%. It has a relevant ETF assets totaling 106.32, uses derivatives (N), and follows a Fixed Income strategy. It has a return month-to-date of +1.25%. As such, it maintains a concentrated presence, focuses on the Investment Grade region, and follows a Fixed Income strategy. It has a NAV tracking error of 2.9817%, a try-to-manage value factor of 1.11%, and a return month-to-date of +1.25%. In order to maintain a specific identifier, the Capital Group US Multi-Sector Income ETF focuses on the Investment Grade region, follows a Corporate strategy, and maintains a NAV tracking error of 2.9817%. It has fund assets totaling 106.32, uses derivatives (N), and follows a Fixed Income strategy. It has a return month-to-date of +1.25%. In summary, the Capital Group US Multi-Sector Income ETF focuses on the Investment Grade region, follows a Corporate strategy, and maintains a N.A. style. It has fund assets totaling 106.32, uses derivatives (N), and follows a Fixed Income strategy. It has a return month-to-date of +1.25%. If you have any other questions, be sure to ask about the Capital Group US Multi-Sector Income ETF. You can find it on the Avantis Core Municipal Fixed Income ETF, focuses on the Investment Grade region, and follows a Fixed Income strategy. It has fund assets totaling 106.32, uses derivatives (N), and follows a Fixed Income strategy. It has a return month-to-date of +1.25%. If you have any other questions, be sure to ask about the Capital Group US Multi-Sector Income ETF. You can find it on the Avantis Core Municipal Fixed Income ETF, focuses on the Investment Grade region, and follows a Fixed Income strategy. It has fund assets totaling 106.32, uses derivatives (N), and follows a Fixed Income strategy. It has a return month-to-date of +1.25%. If you have any other questions, be sure to ask about the Capital Group US Multi-Sector Income ETF. You can find it on the Avantis Core Municipal Fixed Income ETF. It has fund assets totaling 106.32, uses derivatives (N), and follows a Fixed Income strategy. It has a return month-to-date of +1.25%. In response to these questions, the Capital Group US Multi-Sector Income ETF focuses on the Investment Grade region, follows a Corporate strategy, and maintains a N.A. style. It has fund assets totaling 106.32, uses derivatives (N), and follows a Fixed Income strategy. It has a return month-to-date of +1.25%. If you have any other questions, be sure to ask about the Capital Group US Multi-Sector Income ETF. You can find it on the Avantis Core Municipal Fixed Income ETF. It has fund assets totaling 106.32, uses derivatives (N), and follows a Fixed Income strategy. It has a return month-to-date of +1.25%. If you have any other questions, be sure to ask about the Capital Group US Multi-Sector Income ETF. You can find it on the Avantis Core Municipal Fixed Income ETF. It has fund assets totaling 106.32, uses derivatives (N), and follows a Fixed Income strategy. It has a return month-to-date of +1.25%. If you have any other questions, be sure to ask about the Capital Group US Multi-Sector Income ETF. You can find it on the Avantis Core Municipal Fixed Income ETF. It has fund assets totaling 106.32, uses derivatives (N), and follows a Fixed Income strategy. It</t>
+  </si>
+  <si>
+    <t>A balanced strategy that focuses on the JPMorgan Active Bond ETF, including a Fixed Income Directional, Aggregate, and the None style might be what you're looking for. It has an average bid-ask spread of 0.16%, a 30-day volume of 2745, and a return month-to-date of +1.39%. The JPMorgan Active Bond ETF focuses on the Fixed Income Directional strategy, uses assets like Corporate, Corporate, and the Equity it targets. It has a NAV tracking error of 0.5781%, a 30-day volume of 2745, and a return month-to-date of +1.39%. The JPMorgan Active Bond ETF has a fund strategy of Aggregate, total fund assets of 118.96, and an expense ratio of 0.49%. It has a market cap space of 5.05%, and a 30-day volume of 2745. It has a return month-to-date of +1.39%. The JPMorgan Active Bond ETF has a NAV tracking error of 0.5781%, a 30-day volume of 2745, and a return month-to-date of +1.39%. The JPMorgan Active Bond ETF focuses on the Fixed Income Directional strategy, uses assets like Corporate, Corporate, and the Equity it aims to. It has a fund strategy of Aggregate, total fund assets of 118.96, and an expense ratio of 0.49%. It has a market cap space of 5.05%, and a 30-day volume of 2745. It has a return month-to-date of +1.39%. The JPMorgan Active Bond ETF has a fund strategy of Aggregate, total fund assets of 118.96, and an expense ratio of 0.49%. It has a market cap space of 5.05%, target date value of 09/24/18, and a return month-to-date of +1.39%. The JPMorgan Active Bond ETF focuses on the Fixed Income Directional strategy, uses assets like Corporate, Corporate, and the Equity it aims to. It has a fund strategy of Aggregate, total fund assets of 118.96, and an expense ratio of 0.49%. It has a market cap space of 5.05%, target date value of 09/24/18, and a return month-to-date of +1.39%. The JPMorgan Active Bond ETF focuses on the Fixed Income Directional strategy, uses assets like Corporate, Corporate, and the Equity it aims to. It has a fund strategy of Aggregate, total fund assets of 118.96, and an expense ratio of 0.49%. It has a market cap space of 5.05%, target date value of 09/24/18, and a return month-to-date of +1.39%. The JPMorgan Active Bond ETF focuses on the Fixed Income Directional strategy, uses assets like Corporate, Corporate, and the Equity it aims to. It has a fund strategy of Aggregate, total fund assets of 118.96, and an expense ratio of 0.49%. It has a market cap space of 5.05%, target date value of 09/24/18, and a return month-to-date of +1.39%. The JPMorgan Active Bond ETF focuses on the Fixed Income Directional strategy, uses assets like Corporate, Corporate, and the Equity it aims to. It has a fund strategy of Aggregate, total fund assets of 118.96, and an expense ratio of 0.49%. It has a market cap space of 5.05%, target date value of 09/24/18, and a return month-to-date of +1.39%. The JPMorgan Active Bond ETF focuses on the Fixed Income Directional strategy, uses assets like Corporate, Corporate, and the Equity it aims to. It has a fund strategy of Aggregate, total fund assets of 118.96, and an expense ratio of 0.49%. It has a market cap space of 5.05%, target date value of 09/24/18, and a return month-to-date of +1.39%. The JPMorgan Active Bond ETF focuses on the Fixed Income Directional strategy, uses assets like Corporate, Corporate, and the Equity it aims to. It has a fund strategy of Aggregate, total fund assets of 11
+Textbox</t>
+  </si>
+  <si>
+    <t>The CSYU - CSIF IE MSCI USA Tech 125 ESG Universal Blue UCITS ETF focuses on the None region, specifically targeting the N.A. industry, and is associated with the N.A. economic sector. It has a NAV tracking error of None, a 30-day volume of 468724, and a return month-to-date of +1.96%. The Invesco S&amp;P 500 Minimum Variance ETF aims to track the S&amp;P 500 Minimum Volatility Index, using a managed-volatility method. It has a NAV tracking error of None, focuses on the N.A. region, and follows a Economic strategy. The IFETFs key investment objective is to target the None region, uses derivatives (N), and has a NAV tracking error of None. It trades under the ticker SPMV. As for the CSYU - CSIF IE MSCI USA Tech 125 ESG Universal Blue UCITS ETF, its main focus is Thematic, Blend, and its x-bond return month-to-date is +1.96%. It can be contrasted to the CSYU - CSIF IE MSCI USA Tech 125 ESG Universal Blue UCITS ETF. It has a NAV tracking error of None, focuses on the N.A. region, and follows a Economic strategy. However, the IFETFs key investment objective is to target the None region, uses derivatives (N), and has a NAV tracking error of None. It trades under the ticker SPMV. Please note that it has a fund type of ETF, an average bid-ask spread of 0.68%, and a year-to-date return of +1.96%. It can be compared to the CSYU - CSIF IE MSCI USA Tech 125 ESG Universal Blue UCITS ETF. It follows a Economic strategy. However, the IFETFs key Investment Objectives include None. It has a NAV tracking error of None, focuses on the N.A. region, and follows a Economic strategy. However, the IFETFs key investment objective is to target the None region. It uses derivatives (N), has a NAV tracking error of None, and focuses on the N.A. region. It follows a Economic strategy. It has a fund type of ETF, has an average bid-ask spread of 0.68%, and has a year-to-date return of +1.96%. It can be contrasted to the CSYU - CSIF IE MSCI USA Tech 125 ESG Universal Blue UCITS ETF. It follows a Economic strategy. However, the IFETFs key investment objective is to target the None region. It uses derivatives (N), has a NAV tracking error of None, and focuses on the N.A. region. It follows a Economic strategy. However, the IFETFs key investment object is to target the None region. It uses derivatives (N), has a NAV tracking error of None, and focuses on the N.A. region. It follows a Economic strategy. It has a fund type of ETF, has an average bid-ask spread of 0.68%, and has a year-to-date return of +1.96%. It can be compared to the CSYU - CSIF IE MSCI USA Tech 125 ESG Universal Blue UCITS ETF. It follows a Economic strategy. However, the IFETFs key investment objective is to target the None region. It uses derivatives (N), has a NAV tracking error of None, and focuses on the N.A. region. It follows a Economic strategy. It has a fund type of ETF. It has an average bid-ask spread of 0.68%, and has a year-to-date return of +1.96%. It can be contrasted to the CSYU - CSIF IE MSCI USA Tech 125 ESG Universal Blue UCITS ETF. It follows a Economic strategy. However, the IFETFs key investment objective is to target the None region. It uses derivatives (N), has a NAV tracking error of None, and focuses on the N.A. region. It follows a Economic strategy. It has a fund type of ETF. It has an average bid-ask spread of 0.68%, and focuses on the N.A. region. It follows a Economic strategy. It uses derivatives (N) in the same way as it does, uses derivatives (N), has a NAV tracking error of None, and focuses on the N.A. region. It follows a Economic strategy. It follows a Economic strategy. It has a fund type of ETF. It has an average bid-ask spread of 0.68%, and focuses on the N.A. region. It follows a Economic strategy. It uses derivatives (</t>
+  </si>
+  <si>
+    <t>Lora_prompts</t>
+  </si>
+  <si>
+    <t>Lora_portfolio_prompts</t>
+  </si>
+  <si>
+    <t>Lora_modal</t>
+  </si>
+  <si>
+    <t>To create a portfolio of 5 ETFs with equal weights, we can use the Fund's weighting framework. A portfolio consists of three or more actively managed Exchange-Traded Funds that have equal weights based on the underlying indices (in this case, the Russell 1000, S&amp;P 500, and Capped Bond Market). The choice of Fund is based on the investor's risk tolerance, investment goals, and market conditions. This approach ensures that the portfolio follows an equal-weight strategy while maintaining the same level of diversification. There are many ETF options available for such a portfolio construction. Some popular ones include:
+SPDR® MSCI® North America ETF Trust
+SPDR® MSCI USA ETF Trust
+Fukuoka Securities FTSE Japan ETF
+FTSE Japan SMIDIS
+FTSE Japan ETF
+When constructing the portfolio, it's essential to consider the risk tolerance of the investors and the market conditions. For example, during market downturns or significant changes in the investment environment, adjusting the portfolio to maintain equal weight strategies could be beneficial. Additionally, setting clear objectives, such as achieving a certain percentage return over time, can further enhance the portfolio's efficiency. It's recommended to consult with a financial advisor before implementing such a portfolio construction.</t>
+  </si>
+  <si>
+    <t>A portfolio with 3 ETFs investing in the United States would include three ETFs: VFMF, ROUS, and LALT. Each ETF would provide exposure to one or more U.S. stocks based on fundamental analysis. The VFMF invests in large cap stocks, while ROUS invests in mid-cap stocks, and LALT invests in small-cap stocks. Each ETF's primary objective would be to optimize portfolio performance. VFMF is designed to mitigate idiosyncratic risks while also focusing on long-term growth. ROUS, on the other hand, combines robo-advisors with passive investing. LALT is a分散 strategy that invests in short duration bonds. Each ETF's objective will be to minimize volatility. Investors should use a combination of these strategies to achieve their investment objectives. The choice between a passive and active approach will depend on the investor's risk tolerance and investment time horizon.</t>
+  </si>
+  <si>
+    <t>To create a portfolio that combines investment in South Korea and Japan, we can use the 5 ETFs that invest in these countries as a reference. In this example, the portfolio would consist of 5 ETFs that invest in South Korea (SK Food &amp; Beverage), 5 ETFs that invest in Japan (Japan Stock Exchange), 3 ETFs that invest in China Mainland, and 3 ETFs that invest in Japan (Tokyo Stock Exchange).</t>
+  </si>
+  <si>
+    <t>The portfolio would consist of: 5 * (SK Food &amp; Beverage + Japan Stock Exchange + Tokyo Stock Exchange + China Mainland) / (5 + 3 + 1) = 25/12 = 2.74</t>
+  </si>
+  <si>
+    <t>As an AI language model, I cannot make investment decisions, but I can provide you with some guidelines to consider when investing in three growth ETFs, two value ETFs, and one blend ETF. Each ETF has unique investment objectives and risk profiles. For example, the Fidelity All-in-One Growth ETF, the Fidelity All-in-One Growth ETF, the FT Raymond James Multicap Growth Equity ETF, and the Fidelity Fundamental Large Cap Growth ETF have distinct characteristics and performance characteristics. It's essential to do your own due diligence before investing in any of these ETFs to determine whether they align with your investment goals and risk preferences. Additionally, it's important to diversify your investments across different types of ETFs to spread risks and mitigate the impact of any single ETF's underperformance. Consulting with a financial advisor who can help you create a well-diversified portfolio is also crucial.</t>
+  </si>
+  <si>
+    <t>To create a portfolio with returns between 10% and 20%, I will use a multi-fund approach. First, I will select a broad-based fund with a mix of income and capital growth. This will be a multi-factor approach as it's important for investors to have some income generated while maintaining capital preservation. One such option would be the Morningstar U.S. Broad Market Income Strategy ETF (BON).
+Next, I will add a more aggressive component focusing on capital growth. For this, I will supplement the fixed-income ETF with a hedge fund. This ETF is designed to outperform high-quality bonds and can offer a higher level of income compared to traditional bond funds. The Morningstar Global High Yield Hedge Fund (HEDG) ETF (HEDG) provides exposure to global developed market high-yield fixed-income investments. The HEDG ETF will be weighted towards lower credit ratings based on the Morningstar Risk Weighted Credit Score Model, as well as the quality of the underlying assets.
+With both the Morningstar U.S. Broad Market Income Strategy ETF and the HEDG ETF, we aim to provide above-average total return with moderate downside risk. The晨star U.S. Broad Market Income Strategy ETF is an actively managed, multi-factor approach to diversification, while the Morningstar Global High Yield Hedge Fund is a hedge fund. Both the Morningstar U.S. Broad Market Income Strategy ETF and the Morningstar Global High Yield Hedge Fund provide a balance of income and capital preservation. The portfolio's overall allocation will be a blend of value, income and growth stocks to achieve the desired risk profile. The Morningstar U.S. Broad Market Income Strategy ETF is a good choice for investors who want to build a balanced portfolio with above-average returns, moderate downside risk, and a strong balance of asset allocation..</t>
+  </si>
+  <si>
+    <t>To ensure diversification, invest equally into five Value ETFs that focus on the Industrial sector: The S&amp;P Industrial Select Sector SPDR Fund (IXO), iShares MSCI ACWI Industrial ETF (MISC), iShares U.S. Industrials ETF (UIDIA), John Hancock Disciplined Value International Select ETF (JDVI), and Fidelity Industrial Average ETF. This ensures that each ETF's investment approach is designed to capture the return characteristics of the Industrial sector.</t>
+  </si>
+  <si>
+    <t>To create an equal-weighted portfolio of ETFs with 12M yield at least 5%, we first need to select the appropriate ETFs and then adjust the weighting based on the performance of the underlying indices. Assuming that the underlying indices have similar volatility levels (i.e., not having higher or lower volatility), we can use the following formula to select and allocate the ETFs:
+Select the Underlying Index: MarketVantage Russell 1000 Equal Weighted VIX Short Term Futures Index
+Allocate: MarketVantage RIC Equal Weighted VIX Short Term Futures Index (85%) + Invesco S&amp;P 500 Equal Weighted (10%) (10%)
+With this approach, we are allocating 75% of the assets to Invesco RIC Equal Weighted VIX Short Term Futures Index and 15% to Invesco S&amp;P 500 Equal Weighted Index. This strategy aims for yield with minimum level of downside protection as well as potential for upside returns beyond the benchmark. It also minimizes the impact of market fluctuations. However, it's important to note that the choice of the ETF selection method and the weighting of the portfolios may vary based on factors such as liquidity, cost, etc. This scenario does not consider these additional factors. Additionally, the Fund's performance will be closely tied to the performance of the underlying indices.</t>
+  </si>
+  <si>
+    <t>Capital Group Global Multi-Asset Core ETF
+Capital Group US Multi-Sector Income ETF
+Capital Group Global Multi-Asset Core ETF
+Capital Group US Multi-Sector Income ETF
+Capital Group Global Multi-Asset Core ETF
+Capital Group Global Multi-Sector Income ETF
+Capital Group Global Multi-Asset Core ETF
+Capital Group Global Multi-Asset Core ETF
+Capital Group Global Multi-Asset Core ETF
+Capital Group Global Multi-Asset Core ETF
+Each of these ETFs offers investors access to a basket of global or domestic assets, aiming to create diversified portfolios focused on achieving long-term capital gains. Each ETF follows its underlying index and employs active management strategies to achieve its investment objectives. Additionally, some of the funds offer exposure to international markets, as well as alternative diversification techniques. This approach allows investors to gain exposure to a broad range of asset classes, reducing concentration risks while striving for greater portfolio returns.</t>
+  </si>
+  <si>
+    <t>To create an optimal portfolio that invests in the US, we first need to determine the asset allocation for each sector. In the US, the most commonly held sectors include equity, fixed-income, and commodity, which are all equally weighted within the portfolio. In this scenario, the asset allocation will be equal weights. The assets will be invested in the 10 largest sectors: S&amp;P 500, Financials, Industrials, Consumer Cyclical, Consumer Non-Cyclical, Energy, Technology, Utilities. This type of asset allocation minimizes volatility as all securities are equally weighted, while still allowing for potential downside protection. By allocating between equity and fixed-income securities, the portfolio aims to have a moderate risk-return profile. This type of portfolio can provide slightly higher returns compared to a more concentrated portfolio. However, this type of portfolio requires a higher minimum duration of approximately 3 years. Therefore, after optimizing, this type of portfolio would have a Sharpe Ratio of around 0.86%. This means that the portfolio has a positive correlation to the price of one's money relative to the S&amp;P 500 index. This strategy also allows for some downside protection from the US stock market.</t>
+  </si>
+  <si>
+    <t>I'm sorry but as an AI language model, I am not able to execute any technical operations or make trading decisions without access to the individual funds' investment histories and other relevant financial metrics. Additionally, there may be systemic risks and constraints associated with the sub-funds, such as tracking errors or liquidity constraints, that could impact the overall performance of the portfolio. It would be best to consult with a financial advisor who can provide more detailed insights and guidance based on the individual fund's specifics.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F2937"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -342,8 +1027,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,6 +1566,9 @@
       <c r="D10" t="s">
         <v>24</v>
       </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
       <c r="F10" t="s">
         <v>32</v>
       </c>
@@ -929,6 +1629,9 @@
       <c r="D13" t="s">
         <v>21</v>
       </c>
+      <c r="E13" t="s">
+        <v>92</v>
+      </c>
       <c r="F13" t="s">
         <v>36</v>
       </c>
@@ -949,6 +1652,9 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
       <c r="F14" t="s">
         <v>32</v>
       </c>
@@ -969,6 +1675,9 @@
       <c r="D15" t="s">
         <v>33</v>
       </c>
+      <c r="E15" t="s">
+        <v>94</v>
+      </c>
       <c r="F15" t="s">
         <v>32</v>
       </c>
@@ -989,6 +1698,9 @@
       <c r="D16" t="s">
         <v>35</v>
       </c>
+      <c r="E16" t="s">
+        <v>95</v>
+      </c>
       <c r="F16" t="s">
         <v>36</v>
       </c>
@@ -1009,6 +1721,9 @@
       <c r="D17" t="s">
         <v>39</v>
       </c>
+      <c r="E17" t="s">
+        <v>96</v>
+      </c>
       <c r="F17" t="s">
         <v>36</v>
       </c>
@@ -1069,6 +1784,9 @@
       <c r="D20" t="s">
         <v>46</v>
       </c>
+      <c r="E20" t="s">
+        <v>97</v>
+      </c>
       <c r="F20" t="s">
         <v>32</v>
       </c>
@@ -1515,6 +2233,561 @@
       <c r="K42" t="s">
         <v>36</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA5474A-96B3-4AC9-ADBC-0C7A4E66592D}">
+  <dimension ref="A1:AD28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U33" sqref="U33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="144" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="150" customWidth="1"/>
+    <col min="11" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="44.7109375" customWidth="1"/>
+    <col min="16" max="20" width="9.140625" customWidth="1"/>
+    <col min="21" max="21" width="60" customWidth="1"/>
+    <col min="22" max="25" width="9.140625" customWidth="1"/>
+    <col min="26" max="26" width="60" customWidth="1"/>
+    <col min="27" max="30" width="9.140625" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" t="s">
+        <v>104</v>
+      </c>
+      <c r="U1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N2" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R2" t="s">
+        <v>101</v>
+      </c>
+      <c r="S2" t="s">
+        <v>102</v>
+      </c>
+      <c r="U2" t="s">
+        <v>154</v>
+      </c>
+      <c r="V2" t="s">
+        <v>99</v>
+      </c>
+      <c r="W2" t="s">
+        <v>100</v>
+      </c>
+      <c r="X2" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="E28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>